<commit_message>
evidence updates & deltas
</commit_message>
<xml_diff>
--- a/delta2/lib_e/index.xlsx
+++ b/delta2/lib_e/index.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harveywargo/Desktop/GithubProjects/h2w-delta/delta2/lib_e/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FEAE464-CDC8-2841-9CC9-EF3C4EA70117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F590BA3-453D-F440-B763-B83DE1023F92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="760" windowWidth="34480" windowHeight="21580" xr2:uid="{6B3886FC-276B-A343-ADDC-9D0B272B6EC0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="141">
   <si>
     <t>status</t>
   </si>
@@ -410,37 +410,55 @@
     <t>2020-05</t>
   </si>
   <si>
-    <t>processed100</t>
-  </si>
-  <si>
     <t>atk_ttp, htool</t>
   </si>
   <si>
-    <t>202505-adfind.xlsx</t>
-  </si>
-  <si>
-    <t>processed80</t>
-  </si>
-  <si>
     <t>2022-04</t>
   </si>
   <si>
-    <t>processed40</t>
-  </si>
-  <si>
     <t>atk_ttp, htool, atk_chain, sigma, etpro</t>
   </si>
   <si>
-    <t>processed30</t>
-  </si>
-  <si>
     <t>2021-10</t>
   </si>
   <si>
-    <t>processed60</t>
-  </si>
-  <si>
     <t>2021-08</t>
+  </si>
+  <si>
+    <t>processed-61_77</t>
+  </si>
+  <si>
+    <t>processed-32_48</t>
+  </si>
+  <si>
+    <t>processed-47_83</t>
+  </si>
+  <si>
+    <t>processed-54_69</t>
+  </si>
+  <si>
+    <t>processed-10_32</t>
+  </si>
+  <si>
+    <t>processed-35_60</t>
+  </si>
+  <si>
+    <t>processed-28_63</t>
+  </si>
+  <si>
+    <t>https://redcanary.com/blog/threat-detection/getsystem-offsec/</t>
+  </si>
+  <si>
+    <t>2021-01</t>
+  </si>
+  <si>
+    <t>GetSystem</t>
+  </si>
+  <si>
+    <t>adfind.xlsx</t>
+  </si>
+  <si>
+    <t>processed-10_10</t>
   </si>
 </sst>
 </file>
@@ -509,15 +527,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8485BF1E-1098-E146-881D-942226C6C9AA}" name="Table1" displayName="Table1" ref="A1:H49" totalsRowShown="0">
-  <autoFilter ref="A1:H49" xr:uid="{8485BF1E-1098-E146-881D-942226C6C9AA}">
-    <filterColumn colId="4">
-      <filters>
-        <filter val="conti"/>
-        <filter val="ryuk"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8485BF1E-1098-E146-881D-942226C6C9AA}" name="Table1" displayName="Table1" ref="A1:H50" totalsRowShown="0">
+  <autoFilter ref="A1:H50" xr:uid="{8485BF1E-1098-E146-881D-942226C6C9AA}"/>
   <tableColumns count="8">
     <tableColumn id="9" xr3:uid="{E96C26A5-EAFE-BF4D-AFCB-739F293826D0}" name="status"/>
     <tableColumn id="1" xr3:uid="{3EE7B3C7-A063-954C-9545-0F2010F95A61}" name="content"/>
@@ -849,16 +860,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F07DD3A-F1B0-5046-8DBC-C64F8D37E24D}">
-  <dimension ref="A1:H49"/>
+  <dimension ref="A1:H50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B41" sqref="B41"/>
+      <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.83203125" customWidth="1"/>
     <col min="2" max="2" width="34.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.1640625" customWidth="1"/>
     <col min="4" max="4" width="25.83203125" customWidth="1"/>
@@ -894,7 +905,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>20</v>
       </c>
@@ -914,7 +925,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>20</v>
       </c>
@@ -934,7 +945,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>40</v>
       </c>
@@ -952,7 +963,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>20</v>
       </c>
@@ -972,7 +983,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>41</v>
       </c>
@@ -992,7 +1003,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>42</v>
       </c>
@@ -1012,7 +1023,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>20</v>
       </c>
@@ -1032,7 +1043,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>20</v>
       </c>
@@ -1054,7 +1065,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B10" t="s">
         <v>52</v>
@@ -1077,7 +1088,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="B11" t="s">
         <v>52</v>
@@ -1098,7 +1109,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>51</v>
       </c>
@@ -1118,7 +1129,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>50</v>
       </c>
@@ -1138,7 +1149,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>50</v>
       </c>
@@ -1158,7 +1169,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>20</v>
       </c>
@@ -1178,7 +1189,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>71</v>
       </c>
@@ -1198,7 +1209,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>71</v>
       </c>
@@ -1218,7 +1229,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>71</v>
       </c>
@@ -1238,7 +1249,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>71</v>
       </c>
@@ -1258,7 +1269,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="20" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
       <c r="D20" t="s">
         <v>64</v>
       </c>
@@ -1272,7 +1283,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="21" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
       <c r="E21" t="s">
         <v>80</v>
       </c>
@@ -1283,7 +1294,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="22" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
       <c r="E22" t="s">
         <v>39</v>
       </c>
@@ -1294,7 +1305,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="23" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
       <c r="E23" t="s">
         <v>6</v>
       </c>
@@ -1305,7 +1316,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
       <c r="E24" t="s">
         <v>80</v>
       </c>
@@ -1316,7 +1327,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
       <c r="F25" t="s">
         <v>87</v>
       </c>
@@ -1327,7 +1338,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="26" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
       <c r="E26" t="s">
         <v>6</v>
       </c>
@@ -1338,7 +1349,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="27" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
       <c r="E27" t="s">
         <v>91</v>
       </c>
@@ -1347,7 +1358,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="28" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
       <c r="E28" t="s">
         <v>93</v>
       </c>
@@ -1356,7 +1367,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="29" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
       <c r="E29" t="s">
         <v>94</v>
       </c>
@@ -1365,7 +1376,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="30" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
       <c r="E30" t="s">
         <v>94</v>
       </c>
@@ -1374,7 +1385,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="31" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
       <c r="E31" t="s">
         <v>98</v>
       </c>
@@ -1383,7 +1394,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="32" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.2">
       <c r="F32" t="s">
         <v>100</v>
       </c>
@@ -1392,7 +1403,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="33" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E33" t="s">
         <v>98</v>
       </c>
@@ -1401,7 +1412,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F34" t="s">
         <v>103</v>
       </c>
@@ -1412,10 +1423,10 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="B35" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C35" t="s">
         <v>46</v>
@@ -1427,13 +1438,13 @@
         <v>31</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="H35" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F36" t="s">
         <v>106</v>
       </c>
@@ -1442,7 +1453,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F37" t="s">
         <v>106</v>
       </c>
@@ -1453,10 +1464,10 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B38" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C38" t="s">
         <v>46</v>
@@ -1476,10 +1487,10 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B39" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C39" t="s">
         <v>46</v>
@@ -1491,7 +1502,7 @@
         <v>31</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="H39" t="s">
         <v>109</v>
@@ -1499,10 +1510,10 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B40" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C40" t="s">
         <v>46</v>
@@ -1514,13 +1525,19 @@
         <v>31</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="H40" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>130</v>
+      </c>
+      <c r="B41" t="s">
+        <v>126</v>
+      </c>
       <c r="C41" t="s">
         <v>46</v>
       </c>
@@ -1530,12 +1547,14 @@
       <c r="E41" t="s">
         <v>31</v>
       </c>
-      <c r="G41" s="1"/>
+      <c r="G41" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="H41" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="42" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E42" t="s">
         <v>113</v>
       </c>
@@ -1604,7 +1623,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="47" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E47" t="s">
         <v>39</v>
       </c>
@@ -1613,7 +1632,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E48" t="s">
         <v>6</v>
       </c>
@@ -1622,18 +1641,18 @@
         <v>120</v>
       </c>
     </row>
-    <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
+        <v>140</v>
+      </c>
+      <c r="B49" t="s">
         <v>124</v>
-      </c>
-      <c r="B49" t="s">
-        <v>125</v>
       </c>
       <c r="C49" t="s">
         <v>46</v>
       </c>
       <c r="D49" t="s">
-        <v>126</v>
+        <v>139</v>
       </c>
       <c r="F49" t="s">
         <v>122</v>
@@ -1643,6 +1662,17 @@
       </c>
       <c r="H49" t="s">
         <v>121</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F50" t="s">
+        <v>138</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="H50" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
evidence updates & sheet refactors
</commit_message>
<xml_diff>
--- a/delta2/lib_e/index.xlsx
+++ b/delta2/lib_e/index.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harveywargo/Desktop/GithubProjects/h2w-delta/delta2/lib_e/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F590BA3-453D-F440-B763-B83DE1023F92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1E25F32-7908-F748-8BFD-B6E0CC5BBBD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="760" windowWidth="34480" windowHeight="21580" xr2:uid="{6B3886FC-276B-A343-ADDC-9D0B272B6EC0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="147">
   <si>
     <t>status</t>
   </si>
@@ -459,6 +459,24 @@
   </si>
   <si>
     <t>processed-10_10</t>
+  </si>
+  <si>
+    <t>processed-8_34</t>
+  </si>
+  <si>
+    <t>processed-17_30</t>
+  </si>
+  <si>
+    <t>2020-11</t>
+  </si>
+  <si>
+    <t>2020-10</t>
+  </si>
+  <si>
+    <t>processed-17_26</t>
+  </si>
+  <si>
+    <t>processed-19_25</t>
   </si>
 </sst>
 </file>
@@ -864,15 +882,15 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
+      <selection pane="bottomLeft" activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.83203125" customWidth="1"/>
     <col min="2" max="2" width="34.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.1640625" customWidth="1"/>
-    <col min="4" max="4" width="25.83203125" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" customWidth="1"/>
+    <col min="4" max="4" width="20.5" customWidth="1"/>
     <col min="5" max="5" width="24.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.5" customWidth="1"/>
     <col min="7" max="7" width="13.1640625" bestFit="1" customWidth="1"/>
@@ -1564,6 +1582,12 @@
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>141</v>
+      </c>
+      <c r="B43" t="s">
+        <v>126</v>
+      </c>
       <c r="C43" t="s">
         <v>46</v>
       </c>
@@ -1573,12 +1597,20 @@
       <c r="E43" t="s">
         <v>115</v>
       </c>
-      <c r="G43" s="1"/>
+      <c r="G43" s="1" t="s">
+        <v>137</v>
+      </c>
       <c r="H43" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>142</v>
+      </c>
+      <c r="B44" t="s">
+        <v>126</v>
+      </c>
       <c r="C44" t="s">
         <v>46</v>
       </c>
@@ -1588,12 +1620,20 @@
       <c r="E44" t="s">
         <v>115</v>
       </c>
-      <c r="G44" s="1"/>
+      <c r="G44" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="H44" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>145</v>
+      </c>
+      <c r="B45" t="s">
+        <v>126</v>
+      </c>
       <c r="C45" t="s">
         <v>46</v>
       </c>
@@ -1603,12 +1643,20 @@
       <c r="E45" t="s">
         <v>115</v>
       </c>
-      <c r="G45" s="1"/>
+      <c r="G45" s="1" t="s">
+        <v>144</v>
+      </c>
       <c r="H45" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>146</v>
+      </c>
+      <c r="B46" t="s">
+        <v>126</v>
+      </c>
       <c r="C46" t="s">
         <v>46</v>
       </c>
@@ -1618,7 +1666,9 @@
       <c r="E46" t="s">
         <v>115</v>
       </c>
-      <c r="G46" s="1"/>
+      <c r="G46" s="1" t="s">
+        <v>144</v>
+      </c>
       <c r="H46" t="s">
         <v>118</v>
       </c>

</xml_diff>